<commit_message>
Avance de lectura de mallas y asignar especializacion
</commit_message>
<xml_diff>
--- a/Excel_generados/materias_malla.xlsx
+++ b/Excel_generados/materias_malla.xlsx
@@ -5,17 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Desktop\ESPOL\Semestre 7\Metodología de la Investigacion\Proyecto\Git\Repuestos\MetodologiaProyecto\Excel_generados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\GIT\MetodologiaProyecto\Excel_generados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31F0764-EEDE-4260-ABA0-E07D0ABE7BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D69C12-3211-4B2E-BB56-204F22CADE82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="691" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sistemas_multimedia" sheetId="1" r:id="rId1"/>
-    <sheet name="sistemas_de_informacion" sheetId="2" r:id="rId2"/>
-    <sheet name="sistemas_tecnologicos" sheetId="3" r:id="rId3"/>
+    <sheet name="malla_generica" sheetId="4" r:id="rId2"/>
+    <sheet name="sistemas_de_informacion" sheetId="2" r:id="rId3"/>
+    <sheet name="computacion" sheetId="5" r:id="rId4"/>
+    <sheet name="sistemas_tecnologicos" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="208">
   <si>
     <t>Materia</t>
   </si>
@@ -410,6 +412,255 @@
   </si>
   <si>
     <t>FIEC05561</t>
+  </si>
+  <si>
+    <t>COMUNICACIÓN I</t>
+  </si>
+  <si>
+    <t>IDIG2002</t>
+  </si>
+  <si>
+    <t>INDG1001</t>
+  </si>
+  <si>
+    <t>ANÁLISIS Y RESOLUCIÓN DE PROBLEMAS I</t>
+  </si>
+  <si>
+    <t>CÁLCULO DE UNA VARIABLE</t>
+  </si>
+  <si>
+    <t>MATG1001</t>
+  </si>
+  <si>
+    <t>QUÍMICA GENERAL</t>
+  </si>
+  <si>
+    <t>QUIG1001</t>
+  </si>
+  <si>
+    <t>CCPG1001</t>
+  </si>
+  <si>
+    <t>INGLÉS I</t>
+  </si>
+  <si>
+    <t>IDIG1001</t>
+  </si>
+  <si>
+    <t>COMUNICACIÓN II</t>
+  </si>
+  <si>
+    <t>IDIG2003</t>
+  </si>
+  <si>
+    <t>ÁLGEBRA LINEAL</t>
+  </si>
+  <si>
+    <t>MATG1003</t>
+  </si>
+  <si>
+    <t>CÁLCULO DE VARIAS VARIABLES</t>
+  </si>
+  <si>
+    <t>MATG1002</t>
+  </si>
+  <si>
+    <t>FÍSICA I</t>
+  </si>
+  <si>
+    <t>FISG1001</t>
+  </si>
+  <si>
+    <t>BIOG1001</t>
+  </si>
+  <si>
+    <t>INGLÉS II</t>
+  </si>
+  <si>
+    <t>IDIG1002</t>
+  </si>
+  <si>
+    <t>CCPG1004</t>
+  </si>
+  <si>
+    <t>ECUACIONES DIFERENCIALES</t>
+  </si>
+  <si>
+    <t>MATG1004</t>
+  </si>
+  <si>
+    <t>FÍSICA II</t>
+  </si>
+  <si>
+    <t>FISG1002</t>
+  </si>
+  <si>
+    <t>CCPG1005</t>
+  </si>
+  <si>
+    <t>INGLÉS III</t>
+  </si>
+  <si>
+    <t>IDIG1003</t>
+  </si>
+  <si>
+    <t>CIENCIAS DE LA COMPUTACIÓN APLICADAS  A LA SOLUCIÓN DE PROBLEMAS</t>
+  </si>
+  <si>
+    <t>CCPG1007</t>
+  </si>
+  <si>
+    <t>ESTADÍSTICA DESCRIPTIVA</t>
+  </si>
+  <si>
+    <t>ESTG1001</t>
+  </si>
+  <si>
+    <t>MATEMÁTICAS DISCRETAS</t>
+  </si>
+  <si>
+    <t>MATG1005</t>
+  </si>
+  <si>
+    <t>CCPG1006</t>
+  </si>
+  <si>
+    <t>SISTEMA DE BASES DE DATOS</t>
+  </si>
+  <si>
+    <t>TICG1001</t>
+  </si>
+  <si>
+    <t>INGLÉS IV</t>
+  </si>
+  <si>
+    <t>IDIG1004</t>
+  </si>
+  <si>
+    <t>FORMACIÓN COMPLEMENTARIA</t>
+  </si>
+  <si>
+    <t>ESTADÍSTICA INFERENCIAL</t>
+  </si>
+  <si>
+    <t>ESTG1002</t>
+  </si>
+  <si>
+    <t>FUNDAMENTOS DEL DISEÑO DIGITAL</t>
+  </si>
+  <si>
+    <t>CCPG1016</t>
+  </si>
+  <si>
+    <t>ANÁLISIS DE ALGORITMOS</t>
+  </si>
+  <si>
+    <t>CCPG1017</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN DE SISTEMAS</t>
+  </si>
+  <si>
+    <t>CCPG1008</t>
+  </si>
+  <si>
+    <t>INGLÉS V</t>
+  </si>
+  <si>
+    <t>IDIG1005</t>
+  </si>
+  <si>
+    <t>INTRODUCCIÓN A LA GESTIÓN AMBIENTAL</t>
+  </si>
+  <si>
+    <t>ADSG1001</t>
+  </si>
+  <si>
+    <t>METODOLOGÍA DE LA INVESTIGACIÓN EN COMPUTACIÓN</t>
+  </si>
+  <si>
+    <t>CCPG1019</t>
+  </si>
+  <si>
+    <t>REDES DE DATOS &amp;29</t>
+  </si>
+  <si>
+    <t>TLMG1001</t>
+  </si>
+  <si>
+    <t>ORGANIZACIÓN DE COMPUTADORES</t>
+  </si>
+  <si>
+    <t>CCPG1018</t>
+  </si>
+  <si>
+    <t>DISEÑO DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>CCPG1009</t>
+  </si>
+  <si>
+    <t>EMPRENDIMIENTO E INNOVACIÓN &amp;34</t>
+  </si>
+  <si>
+    <t>ADMG2001</t>
+  </si>
+  <si>
+    <t>SEGURIDAD DE LA INFORMACIÓN</t>
+  </si>
+  <si>
+    <t>CCPG1003</t>
+  </si>
+  <si>
+    <t>SOFG1001</t>
+  </si>
+  <si>
+    <t>CCPG1010</t>
+  </si>
+  <si>
+    <t>CCPG1011</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN DE PROYECTOS INFORMÁTICOS</t>
+  </si>
+  <si>
+    <t>CCPG1012</t>
+  </si>
+  <si>
+    <t>INTERACCIÓN HUMANO COMPUTADOR</t>
+  </si>
+  <si>
+    <t>CCPG1023</t>
+  </si>
+  <si>
+    <t>SOFG1002</t>
+  </si>
+  <si>
+    <t>CCPG1013</t>
+  </si>
+  <si>
+    <t>ITINERARIO</t>
+  </si>
+  <si>
+    <t>CCPG1014</t>
+  </si>
+  <si>
+    <t>SISTEMAS DISTRIBUIDOS</t>
+  </si>
+  <si>
+    <t>CCPG1015</t>
+  </si>
+  <si>
+    <t>SOFG1003</t>
+  </si>
+  <si>
+    <t>MATERIA INTEGRADORA DE INGENIERÍA EN COMPUTACIÓN &amp;50</t>
+  </si>
+  <si>
+    <t>CCPG1026</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -419,7 +670,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,6 +688,12 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -470,7 +727,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -493,18 +750,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -791,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D55" sqref="A50:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,11 +1076,11 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15">
-        <v>4</v>
+      <c r="C2" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -839,8 +1093,8 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="15">
-        <v>4</v>
+      <c r="C3" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -853,8 +1107,8 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15">
-        <v>5</v>
+      <c r="C4" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -867,8 +1121,8 @@
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="15">
-        <v>4</v>
+      <c r="C5" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -878,11 +1132,11 @@
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="15">
-        <v>2</v>
+      <c r="C6" s="19" t="s">
+        <v>207</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -892,11 +1146,11 @@
       <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="21">
-        <v>5</v>
+      <c r="C7" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -909,7 +1163,7 @@
       <c r="B8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="2">
@@ -921,11 +1175,11 @@
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="21">
-        <v>5</v>
+      <c r="C9" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -938,7 +1192,7 @@
       <c r="B10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2">
@@ -952,7 +1206,7 @@
       <c r="B11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="2">
@@ -966,7 +1220,7 @@
       <c r="B12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="20" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="2">
@@ -980,7 +1234,7 @@
       <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="2">
@@ -994,7 +1248,7 @@
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="2">
@@ -1009,7 +1263,7 @@
       <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2">
@@ -1023,7 +1277,7 @@
       <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="2">
@@ -1037,7 +1291,7 @@
       <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="2">
@@ -1051,7 +1305,7 @@
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="2">
@@ -1062,11 +1316,11 @@
       <c r="A19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="15">
-        <v>2</v>
+      <c r="C19" s="19" t="s">
+        <v>207</v>
       </c>
       <c r="D19" s="2">
         <v>3</v>
@@ -1079,7 +1333,7 @@
       <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="2">
@@ -1091,11 +1345,11 @@
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
+      <c r="C21" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D21" s="2">
         <v>4</v>
@@ -1108,7 +1362,7 @@
       <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="2">
@@ -1122,7 +1376,7 @@
       <c r="B23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2">
@@ -1136,7 +1390,7 @@
       <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="2">
@@ -1150,7 +1404,7 @@
       <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="2">
@@ -1171,7 +1425,7 @@
       <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="2">
@@ -1185,7 +1439,7 @@
       <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="2">
@@ -1199,7 +1453,7 @@
       <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="2">
@@ -1210,11 +1464,11 @@
       <c r="A29" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="2">
-        <v>5</v>
+      <c r="C29" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D29" s="2">
         <v>5</v>
@@ -1227,7 +1481,7 @@
       <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="2">
@@ -1241,7 +1495,7 @@
       <c r="B31" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="2">
@@ -1262,7 +1516,7 @@
       <c r="B32" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="2">
@@ -1276,7 +1530,7 @@
       <c r="B33" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D33" s="2">
@@ -1290,7 +1544,7 @@
       <c r="B34" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="2">
@@ -1304,7 +1558,7 @@
       <c r="B35" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D35" s="2">
@@ -1318,7 +1572,7 @@
       <c r="B36" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="2">
@@ -1332,7 +1586,7 @@
       <c r="B37" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="2">
@@ -1346,7 +1600,7 @@
       <c r="B38" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D38" s="2">
@@ -1360,7 +1614,7 @@
       <c r="B39" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D39" s="2">
@@ -1374,7 +1628,7 @@
       <c r="B40" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="2">
@@ -1388,7 +1642,7 @@
       <c r="B41" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D41" s="2">
@@ -1402,7 +1656,7 @@
       <c r="B42" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D42" s="2">
@@ -1416,7 +1670,7 @@
       <c r="B43" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D43" s="2">
@@ -1430,7 +1684,7 @@
       <c r="B44" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D44" s="2">
@@ -1444,7 +1698,7 @@
       <c r="B45" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="2">
@@ -1458,7 +1712,7 @@
       <c r="B46" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="2">
@@ -1472,7 +1726,7 @@
       <c r="B47" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D47" s="2">
@@ -1486,8 +1740,8 @@
       <c r="B48" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="2">
-        <v>3</v>
+      <c r="C48" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D48" s="2">
         <v>8</v>
@@ -1500,8 +1754,8 @@
       <c r="B49" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="2">
-        <v>4</v>
+      <c r="C49" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D49" s="2">
         <v>8</v>
@@ -1514,7 +1768,7 @@
       <c r="B50" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D50" s="2">
@@ -1528,7 +1782,7 @@
       <c r="B51" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D51" s="2">
@@ -1542,8 +1796,8 @@
       <c r="B52" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="2">
-        <v>4</v>
+      <c r="C52" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D52" s="2">
         <v>9</v>
@@ -1556,8 +1810,8 @@
       <c r="B53" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="2">
-        <v>4</v>
+      <c r="C53" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D53" s="2">
         <v>9</v>
@@ -1570,8 +1824,8 @@
       <c r="B54" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="2">
-        <v>4</v>
+      <c r="C54" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D54" s="2">
         <v>9</v>
@@ -1584,8 +1838,8 @@
       <c r="B55" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="2">
-        <v>4</v>
+      <c r="C55" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D55" s="2">
         <v>9</v>
@@ -1598,8 +1852,8 @@
       <c r="B56" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="2">
-        <v>3</v>
+      <c r="C56" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D56" s="2">
         <v>10</v>
@@ -1612,8 +1866,8 @@
       <c r="B57" t="s">
         <v>106</v>
       </c>
-      <c r="C57" s="2">
-        <v>3</v>
+      <c r="C57" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D57" s="2">
         <v>10</v>
@@ -1626,8 +1880,8 @@
       <c r="B58" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="2">
-        <v>3</v>
+      <c r="C58" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D58" s="2">
         <v>10</v>
@@ -1639,11 +1893,445 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB4641-2A61-465F-AFAB-A69356144125}">
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="56.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E78F711-ACAF-40F8-B422-D160A62A92F2}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,11 +2359,11 @@
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15">
-        <v>4</v>
+      <c r="C2" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -1688,8 +2376,8 @@
       <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="15">
-        <v>4</v>
+      <c r="C3" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -1702,8 +2390,8 @@
       <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15">
-        <v>5</v>
+      <c r="C4" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -1716,8 +2404,8 @@
       <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="15">
-        <v>4</v>
+      <c r="C5" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -1727,11 +2415,11 @@
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="15">
-        <v>2</v>
+      <c r="C6" s="19" t="s">
+        <v>207</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -1741,11 +2429,11 @@
       <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="21">
-        <v>5</v>
+      <c r="C7" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1758,7 +2446,7 @@
       <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="2">
@@ -1769,11 +2457,11 @@
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="21">
-        <v>5</v>
+      <c r="C9" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -1786,7 +2474,7 @@
       <c r="B10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2">
@@ -1800,7 +2488,7 @@
       <c r="B11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="2">
@@ -1814,7 +2502,7 @@
       <c r="B12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="20" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="2">
@@ -1828,7 +2516,7 @@
       <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="2">
@@ -1842,7 +2530,7 @@
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="2">
@@ -1856,7 +2544,7 @@
       <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2">
@@ -1870,7 +2558,7 @@
       <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="2">
@@ -1884,7 +2572,7 @@
       <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="2">
@@ -1898,7 +2586,7 @@
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="2">
@@ -1909,11 +2597,11 @@
       <c r="A19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="15">
-        <v>2</v>
+      <c r="C19" s="19" t="s">
+        <v>207</v>
       </c>
       <c r="D19" s="2">
         <v>3</v>
@@ -1926,7 +2614,7 @@
       <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="2">
@@ -1937,11 +2625,11 @@
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
+      <c r="C21" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D21" s="2">
         <v>4</v>
@@ -1954,7 +2642,7 @@
       <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="2">
@@ -1968,7 +2656,7 @@
       <c r="B23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2">
@@ -1982,7 +2670,7 @@
       <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="2">
@@ -1996,7 +2684,7 @@
       <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="2">
@@ -2010,7 +2698,7 @@
       <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="2">
@@ -2024,7 +2712,7 @@
       <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="2">
@@ -2038,7 +2726,7 @@
       <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="2">
@@ -2049,11 +2737,11 @@
       <c r="A29" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="2">
-        <v>5</v>
+      <c r="C29" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D29" s="2">
         <v>5</v>
@@ -2066,7 +2754,7 @@
       <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="2">
@@ -2080,7 +2768,7 @@
       <c r="B31" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="2">
@@ -2094,8 +2782,8 @@
       <c r="B32" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="2">
-        <v>5</v>
+      <c r="C32" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D32" s="2">
         <v>6</v>
@@ -2108,7 +2796,7 @@
       <c r="B33" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D33" s="2">
@@ -2122,7 +2810,7 @@
       <c r="B34" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="2">
@@ -2136,7 +2824,7 @@
       <c r="B35" t="s">
         <v>116</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D35" s="2">
@@ -2150,7 +2838,7 @@
       <c r="B36" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="2">
@@ -2164,7 +2852,7 @@
       <c r="B37" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="2">
@@ -2178,7 +2866,7 @@
       <c r="B38" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D38" s="2">
@@ -2192,7 +2880,7 @@
       <c r="B39" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D39" s="2">
@@ -2206,7 +2894,7 @@
       <c r="B40" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="2">
@@ -2220,7 +2908,7 @@
       <c r="B41" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D41" s="2">
@@ -2234,7 +2922,7 @@
       <c r="B42" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D42" s="2">
@@ -2248,7 +2936,7 @@
       <c r="B43" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D43" s="2">
@@ -2262,7 +2950,7 @@
       <c r="B44" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D44" s="2">
@@ -2276,7 +2964,7 @@
       <c r="B45" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="2">
@@ -2290,7 +2978,7 @@
       <c r="B46" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="2">
@@ -2304,7 +2992,7 @@
       <c r="B47" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D47" s="2">
@@ -2318,8 +3006,8 @@
       <c r="B48" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="2">
-        <v>3</v>
+      <c r="C48" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D48" s="2">
         <v>8</v>
@@ -2332,8 +3020,8 @@
       <c r="B49" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="2">
-        <v>4</v>
+      <c r="C49" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D49" s="2">
         <v>8</v>
@@ -2346,7 +3034,7 @@
       <c r="B50" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D50" s="2">
@@ -2360,7 +3048,7 @@
       <c r="B51" t="s">
         <v>114</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D51" s="2">
@@ -2374,8 +3062,8 @@
       <c r="B52" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="2">
-        <v>4</v>
+      <c r="C52" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D52" s="2">
         <v>9</v>
@@ -2388,8 +3076,8 @@
       <c r="B53" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="2">
-        <v>4</v>
+      <c r="C53" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D53" s="2">
         <v>9</v>
@@ -2402,8 +3090,8 @@
       <c r="B54" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="2">
-        <v>4</v>
+      <c r="C54" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D54" s="2">
         <v>9</v>
@@ -2416,8 +3104,8 @@
       <c r="B55" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="2">
-        <v>4</v>
+      <c r="C55" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D55" s="2">
         <v>9</v>
@@ -2430,8 +3118,8 @@
       <c r="B56" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="2">
-        <v>3</v>
+      <c r="C56" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D56" s="2">
         <v>10</v>
@@ -2444,8 +3132,8 @@
       <c r="B57" t="s">
         <v>106</v>
       </c>
-      <c r="C57" s="2">
-        <v>3</v>
+      <c r="C57" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D57" s="2">
         <v>10</v>
@@ -2458,8 +3146,8 @@
       <c r="B58" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="2">
-        <v>3</v>
+      <c r="C58" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D58" s="2">
         <v>10</v>
@@ -2470,12 +3158,788 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7478C8-4406-4F0C-8240-457562D314C6}">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D25" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" t="s">
+        <v>170</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" t="s">
+        <v>176</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>179</v>
+      </c>
+      <c r="B32" t="s">
+        <v>180</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>183</v>
+      </c>
+      <c r="B34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>185</v>
+      </c>
+      <c r="B35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>187</v>
+      </c>
+      <c r="B36" t="s">
+        <v>188</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" t="s">
+        <v>192</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>166</v>
+      </c>
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D41" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42" t="s">
+        <v>195</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>196</v>
+      </c>
+      <c r="B43" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
+        <v>198</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>199</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>200</v>
+      </c>
+      <c r="B46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D47" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>202</v>
+      </c>
+      <c r="B49" t="s">
+        <v>203</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" t="s">
+        <v>204</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>200</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>166</v>
+      </c>
+      <c r="B52" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D52" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54" t="s">
+        <v>206</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="15">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C240FC97-6CF8-40B5-9196-C3AB7E86894A}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2503,11 +3967,11 @@
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15">
-        <v>4</v>
+      <c r="C2" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -2520,8 +3984,8 @@
       <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="15">
-        <v>4</v>
+      <c r="C3" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -2534,8 +3998,8 @@
       <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15">
-        <v>5</v>
+      <c r="C4" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -2548,8 +4012,8 @@
       <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="15">
-        <v>4</v>
+      <c r="C5" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -2559,11 +4023,11 @@
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="15">
-        <v>2</v>
+      <c r="C6" s="19" t="s">
+        <v>207</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -2573,11 +4037,11 @@
       <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="21">
-        <v>5</v>
+      <c r="C7" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -2590,7 +4054,7 @@
       <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="2">
@@ -2601,11 +4065,11 @@
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="21">
-        <v>5</v>
+      <c r="C9" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -2618,7 +4082,7 @@
       <c r="B10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2">
@@ -2632,7 +4096,7 @@
       <c r="B11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="2">
@@ -2646,7 +4110,7 @@
       <c r="B12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="20" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="2">
@@ -2660,7 +4124,7 @@
       <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="2">
@@ -2674,7 +4138,7 @@
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="2">
@@ -2688,7 +4152,7 @@
       <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2">
@@ -2702,7 +4166,7 @@
       <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="2">
@@ -2716,7 +4180,7 @@
       <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="2">
@@ -2730,7 +4194,7 @@
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="2">
@@ -2741,11 +4205,11 @@
       <c r="A19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="15">
-        <v>2</v>
+      <c r="C19" s="19" t="s">
+        <v>207</v>
       </c>
       <c r="D19" s="2">
         <v>3</v>
@@ -2758,7 +4222,7 @@
       <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="2">
@@ -2769,11 +4233,11 @@
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
+      <c r="C21" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D21" s="2">
         <v>4</v>
@@ -2786,7 +4250,7 @@
       <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="2">
@@ -2800,7 +4264,7 @@
       <c r="B23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2">
@@ -2814,7 +4278,7 @@
       <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="2">
@@ -2828,7 +4292,7 @@
       <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="2">
@@ -2842,7 +4306,7 @@
       <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="2">
@@ -2856,7 +4320,7 @@
       <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="2">
@@ -2870,7 +4334,7 @@
       <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="2">
@@ -2881,11 +4345,11 @@
       <c r="A29" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="2">
-        <v>5</v>
+      <c r="C29" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D29" s="2">
         <v>5</v>
@@ -2898,7 +4362,7 @@
       <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="2">
@@ -2912,7 +4376,7 @@
       <c r="B31" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="2">
@@ -2926,8 +4390,8 @@
       <c r="B32" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="2">
-        <v>5</v>
+      <c r="C32" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="D32" s="2">
         <v>6</v>
@@ -2940,7 +4404,7 @@
       <c r="B33" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D33" s="2">
@@ -2951,11 +4415,11 @@
       <c r="A34" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="2">
-        <v>3</v>
+      <c r="C34" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D34" s="2">
         <v>6</v>
@@ -2968,7 +4432,7 @@
       <c r="B35" t="s">
         <v>120</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D35" s="2">
@@ -2982,7 +4446,7 @@
       <c r="B36" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="2">
@@ -2996,7 +4460,7 @@
       <c r="B37" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="2">
@@ -3010,7 +4474,7 @@
       <c r="B38" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D38" s="2">
@@ -3024,7 +4488,7 @@
       <c r="B39" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D39" s="2">
@@ -3038,7 +4502,7 @@
       <c r="B40" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="2">
@@ -3049,11 +4513,11 @@
       <c r="A41" t="s">
         <v>121</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="2">
-        <v>3</v>
+      <c r="C41" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D41" s="2">
         <v>7</v>
@@ -3066,7 +4530,7 @@
       <c r="B42" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D42" s="2">
@@ -3080,7 +4544,7 @@
       <c r="B43" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D43" s="2">
@@ -3094,7 +4558,7 @@
       <c r="B44" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D44" s="2">
@@ -3108,7 +4572,7 @@
       <c r="B45" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="2">
@@ -3122,7 +4586,7 @@
       <c r="B46" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="2">
@@ -3133,11 +4597,11 @@
       <c r="A47" t="s">
         <v>123</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C47" s="2">
-        <v>6</v>
+      <c r="C47" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="D47" s="2">
         <v>8</v>
@@ -3150,8 +4614,8 @@
       <c r="B48" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="2">
-        <v>3</v>
+      <c r="C48" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D48" s="2">
         <v>8</v>
@@ -3164,8 +4628,8 @@
       <c r="B49" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="2">
-        <v>4</v>
+      <c r="C49" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D49" s="2">
         <v>8</v>
@@ -3178,7 +4642,7 @@
       <c r="B50" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D50" s="2">
@@ -3192,7 +4656,7 @@
       <c r="B51" t="s">
         <v>114</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D51" s="2">
@@ -3206,8 +4670,8 @@
       <c r="B52" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="2">
-        <v>4</v>
+      <c r="C52" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D52" s="2">
         <v>9</v>
@@ -3220,8 +4684,8 @@
       <c r="B53" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="2">
-        <v>4</v>
+      <c r="C53" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D53" s="2">
         <v>9</v>
@@ -3234,8 +4698,8 @@
       <c r="B54" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="2">
-        <v>4</v>
+      <c r="C54" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D54" s="2">
         <v>9</v>
@@ -3248,8 +4712,8 @@
       <c r="B55" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="2">
-        <v>4</v>
+      <c r="C55" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D55" s="2">
         <v>9</v>
@@ -3262,8 +4726,8 @@
       <c r="B56" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="2">
-        <v>3</v>
+      <c r="C56" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D56" s="2">
         <v>10</v>
@@ -3276,8 +4740,8 @@
       <c r="B57" t="s">
         <v>106</v>
       </c>
-      <c r="C57" s="2">
-        <v>3</v>
+      <c r="C57" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D57" s="2">
         <v>10</v>
@@ -3290,8 +4754,8 @@
       <c r="B58" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="2">
-        <v>3</v>
+      <c r="C58" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D58" s="2">
         <v>10</v>

</xml_diff>

<commit_message>
Cambios en eficiencia e integradora
</commit_message>
<xml_diff>
--- a/Excel_generados/materias_malla.xlsx
+++ b/Excel_generados/materias_malla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Desktop\ESPOL\Semestre 7\Metodología de la Investigacion\Proyecto\Git\Repuestos\MetodologiaProyecto\Excel_generados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Desktop\ESPOL\Semestre 7\Metodología de la Investigacion\Proyecto\Git\MetodologiaProyecto\Excel_generados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31F0764-EEDE-4260-ABA0-E07D0ABE7BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748EA85A-7302-4FC5-B370-32AF71DE4763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -792,7 +792,7 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,7 +1642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E78F711-ACAF-40F8-B422-D160A62A92F2}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>